<commit_message>
no sé, si dañé algo perdón
</commit_message>
<xml_diff>
--- a/src/main/resources/ProductosBusqueda.xlsx
+++ b/src/main/resources/ProductosBusqueda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natalia\Desktop\Universidad_6\Calidad\STORE_2511\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1BA621-187E-441E-9663-F77364B2CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC57356-949A-4327-91A0-D71C8051292E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{012D003F-895D-40AA-BDEA-D8500F49FC76}"/>
   </bookViews>
@@ -83,16 +83,16 @@
     <t>Mac</t>
   </si>
   <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
     <t>iMac</t>
-  </si>
-  <si>
-    <t>ExpectedResult</t>
-  </si>
-  <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>SUCCESS</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="63" x14ac:dyDescent="0.25">
@@ -510,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="63" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
         <v>-1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -568,13 +568,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>